<commit_message>
EFO/DO december 2022 release
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package_phenOncoX/phenOncoX/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F25405-E9B4-4A4D-BF09-C51A96275692}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1A1E87-52BD-D74D-8F0B-F93EF0B4C9BA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -120,10 +120,10 @@
     <t>Hereditary cancer phenotypes/syndromes</t>
   </si>
   <si>
-    <t>v3.48.0</t>
-  </si>
-  <si>
-    <t>v2022-11-30</t>
+    <t>v3.49.0</t>
+  </si>
+  <si>
+    <t>v2022-12-15</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DO/EFO jan 2023 update
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1A1E87-52BD-D74D-8F0B-F93EF0B4C9BA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372A8D83-1DFA-A947-B0C1-BC88FBF591A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -120,10 +120,10 @@
     <t>Hereditary cancer phenotypes/syndromes</t>
   </si>
   <si>
-    <t>v3.49.0</t>
-  </si>
-  <si>
-    <t>v2022-12-15</t>
+    <t>v2023-01-31</t>
+  </si>
+  <si>
+    <t>v3.50.0</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -606,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
DO + EFO feb 2023 update
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372A8D83-1DFA-A947-B0C1-BC88FBF591A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE5446A-566F-3749-8207-23961D17476C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="5940" yWindow="2780" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="phen_oncox" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,10 +120,10 @@
     <t>Hereditary cancer phenotypes/syndromes</t>
   </si>
   <si>
-    <t>v2023-01-31</t>
-  </si>
-  <si>
-    <t>v3.50.0</t>
+    <t>v3.51.0</t>
+  </si>
+  <si>
+    <t>v2023-02-27</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -606,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
EFO 3.52, DO April 2023
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__phenOncoX/phenOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE5446A-566F-3749-8207-23961D17476C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCB8F0E-F9B7-8C4E-88DE-99C13D9F4DD4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5940" yWindow="2780" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -120,10 +120,10 @@
     <t>Hereditary cancer phenotypes/syndromes</t>
   </si>
   <si>
-    <t>v3.51.0</t>
-  </si>
-  <si>
-    <t>v2023-02-27</t>
+    <t>v2023-04-01</t>
+  </si>
+  <si>
+    <t>v3.52.0</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -606,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>

</xml_diff>